<commit_message>
new plot and change in xlsx file
</commit_message>
<xml_diff>
--- a/data/ADHD_MC.xlsx
+++ b/data/ADHD_MC.xlsx
@@ -526,15 +526,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -708,10 +708,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ108"/>
+  <dimension ref="A1:AJ112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH16" activeCellId="0" sqref="AH16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,13 +816,13 @@
       <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -923,13 +923,13 @@
       <c r="AF2" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
-      <c r="AH2" s="0" t="n">
+      <c r="AH2" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI2" s="0" t="n">
+      <c r="AI2" s="1" t="n">
         <v>1.19</v>
       </c>
-      <c r="AJ2" s="0" t="n">
+      <c r="AJ2" s="1" t="n">
         <v>4.67</v>
       </c>
     </row>
@@ -1030,13 +1030,13 @@
       <c r="AF3" s="2" t="n">
         <v>-0.0264900662251655</v>
       </c>
-      <c r="AH3" s="0" t="n">
+      <c r="AH3" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="AI3" s="0" t="n">
+      <c r="AI3" s="1" t="n">
         <v>-0.84</v>
       </c>
-      <c r="AJ3" s="0" t="n">
+      <c r="AJ3" s="1" t="n">
         <v>-1.46</v>
       </c>
     </row>
@@ -1137,13 +1137,13 @@
       <c r="AF4" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
-      <c r="AH4" s="0" t="n">
+      <c r="AH4" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI4" s="0" t="n">
+      <c r="AI4" s="1" t="n">
         <v>1.31</v>
       </c>
-      <c r="AJ4" s="0" t="n">
+      <c r="AJ4" s="1" t="n">
         <v>1.91</v>
       </c>
     </row>
@@ -1244,13 +1244,13 @@
       <c r="AF5" s="2" t="n">
         <v>3.41721854304636</v>
       </c>
-      <c r="AH5" s="0" t="n">
+      <c r="AH5" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="AI5" s="0" t="n">
+      <c r="AI5" s="1" t="n">
         <v>-0.4</v>
       </c>
-      <c r="AJ5" s="0" t="n">
+      <c r="AJ5" s="1" t="n">
         <v>-1.27</v>
       </c>
     </row>
@@ -1351,13 +1351,13 @@
       <c r="AF6" s="2" t="n">
         <v>2.62251655629139</v>
       </c>
-      <c r="AH6" s="0" t="n">
+      <c r="AH6" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="AI6" s="0" t="n">
+      <c r="AI6" s="1" t="n">
         <v>-1.49</v>
       </c>
-      <c r="AJ6" s="0" t="n">
+      <c r="AJ6" s="1" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -1458,13 +1458,13 @@
       <c r="AF7" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
-      <c r="AH7" s="0" t="n">
+      <c r="AH7" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="AI7" s="0" t="n">
+      <c r="AI7" s="1" t="n">
         <v>2.32</v>
       </c>
-      <c r="AJ7" s="0" t="n">
+      <c r="AJ7" s="1" t="n">
         <v>1.93</v>
       </c>
     </row>
@@ -1565,13 +1565,13 @@
       <c r="AF8" s="2" t="n">
         <v>3.1523178807947</v>
       </c>
-      <c r="AH8" s="0" t="n">
+      <c r="AH8" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI8" s="0" t="n">
+      <c r="AI8" s="1" t="n">
         <v>1.93</v>
       </c>
-      <c r="AJ8" s="0" t="n">
+      <c r="AJ8" s="1" t="n">
         <v>4.95</v>
       </c>
     </row>
@@ -1672,13 +1672,13 @@
       <c r="AF9" s="2" t="n">
         <v>3.81456953642384</v>
       </c>
-      <c r="AH9" s="0" t="n">
+      <c r="AH9" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="AI9" s="0" t="n">
+      <c r="AI9" s="1" t="n">
         <v>0.88</v>
       </c>
-      <c r="AJ9" s="0" t="n">
+      <c r="AJ9" s="1" t="n">
         <v>3.92</v>
       </c>
     </row>
@@ -1779,13 +1779,13 @@
       <c r="AF10" s="2" t="n">
         <v>1.43046357615894</v>
       </c>
-      <c r="AH10" s="0" t="n">
+      <c r="AH10" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="AI10" s="0" t="n">
+      <c r="AI10" s="1" t="n">
         <v>-1.31</v>
       </c>
-      <c r="AJ10" s="0" t="n">
+      <c r="AJ10" s="1" t="n">
         <v>0.18</v>
       </c>
     </row>
@@ -1886,13 +1886,13 @@
       <c r="AF11" s="2" t="n">
         <v>1.03311258278146</v>
       </c>
-      <c r="AH11" s="0" t="n">
+      <c r="AH11" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="AI11" s="0" t="n">
+      <c r="AI11" s="1" t="n">
         <v>-1.24</v>
       </c>
-      <c r="AJ11" s="0" t="n">
+      <c r="AJ11" s="1" t="n">
         <v>-0.88</v>
       </c>
     </row>
@@ -1993,13 +1993,13 @@
       <c r="AF12" s="2" t="n">
         <v>3.01986754966887</v>
       </c>
-      <c r="AH12" s="0" t="n">
+      <c r="AH12" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI12" s="0" t="n">
+      <c r="AI12" s="1" t="n">
         <v>0.45</v>
       </c>
-      <c r="AJ12" s="0" t="n">
+      <c r="AJ12" s="1" t="n">
         <v>2.25</v>
       </c>
     </row>
@@ -2100,13 +2100,13 @@
       <c r="AF13" s="2" t="n">
         <v>1.56291390728477</v>
       </c>
-      <c r="AH13" s="0" t="n">
+      <c r="AH13" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI13" s="0" t="n">
+      <c r="AI13" s="1" t="n">
         <v>2.24</v>
       </c>
-      <c r="AJ13" s="0" t="n">
+      <c r="AJ13" s="1" t="n">
         <v>3.11</v>
       </c>
     </row>
@@ -2207,13 +2207,13 @@
       <c r="AF14" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
-      <c r="AH14" s="0" t="n">
+      <c r="AH14" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI14" s="0" t="n">
+      <c r="AI14" s="1" t="n">
         <v>-1.15</v>
       </c>
-      <c r="AJ14" s="0" t="n">
+      <c r="AJ14" s="1" t="n">
         <v>-0.39</v>
       </c>
     </row>
@@ -2314,13 +2314,13 @@
       <c r="AF15" s="2" t="n">
         <v>2.35761589403974</v>
       </c>
-      <c r="AH15" s="0" t="n">
+      <c r="AH15" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AI15" s="0" t="n">
+      <c r="AI15" s="1" t="n">
         <v>2.21</v>
       </c>
-      <c r="AJ15" s="0" t="n">
+      <c r="AJ15" s="1" t="n">
         <v>4.89</v>
       </c>
     </row>
@@ -2421,13 +2421,13 @@
       <c r="AF16" s="2" t="n">
         <v>3.41721854304636</v>
       </c>
-      <c r="AH16" s="0" t="n">
+      <c r="AH16" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI16" s="0" t="n">
+      <c r="AI16" s="1" t="n">
         <v>-0.73</v>
       </c>
-      <c r="AJ16" s="0" t="n">
+      <c r="AJ16" s="1" t="n">
         <v>-0.88</v>
       </c>
     </row>
@@ -2528,13 +2528,13 @@
       <c r="AF17" s="2" t="n">
         <v>1.03311258278146</v>
       </c>
-      <c r="AH17" s="0" t="n">
+      <c r="AH17" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="AI17" s="0" t="n">
+      <c r="AI17" s="1" t="n">
         <v>2.32</v>
       </c>
-      <c r="AJ17" s="0" t="n">
+      <c r="AJ17" s="1" t="n">
         <v>2.63</v>
       </c>
     </row>
@@ -2635,13 +2635,13 @@
       <c r="AF18" s="2" t="n">
         <v>0.768211920529802</v>
       </c>
-      <c r="AH18" s="0" t="n">
+      <c r="AH18" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI18" s="0" t="n">
+      <c r="AI18" s="1" t="n">
         <v>-0.81</v>
       </c>
-      <c r="AJ18" s="0" t="n">
+      <c r="AJ18" s="1" t="n">
         <v>-0.65</v>
       </c>
     </row>
@@ -2742,13 +2742,13 @@
       <c r="AF19" s="2" t="n">
         <v>1.96026490066225</v>
       </c>
-      <c r="AH19" s="0" t="n">
+      <c r="AH19" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI19" s="0" t="n">
+      <c r="AI19" s="1" t="n">
         <v>0.33</v>
       </c>
-      <c r="AJ19" s="0" t="n">
+      <c r="AJ19" s="1" t="n">
         <v>1.08</v>
       </c>
     </row>
@@ -2849,13 +2849,13 @@
       <c r="AF20" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
-      <c r="AH20" s="0" t="n">
+      <c r="AH20" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="AI20" s="0" t="n">
+      <c r="AI20" s="1" t="n">
         <v>-0.06</v>
       </c>
-      <c r="AJ20" s="0" t="n">
+      <c r="AJ20" s="1" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -2956,13 +2956,13 @@
       <c r="AF21" s="2" t="n">
         <v>1.6953642384106</v>
       </c>
-      <c r="AH21" s="0" t="n">
+      <c r="AH21" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI21" s="0" t="n">
+      <c r="AI21" s="1" t="n">
         <v>0.41</v>
       </c>
-      <c r="AJ21" s="0" t="n">
+      <c r="AJ21" s="1" t="n">
         <v>3.84</v>
       </c>
     </row>
@@ -3063,13 +3063,13 @@
       <c r="AF22" s="2" t="n">
         <v>4.34437086092715</v>
       </c>
-      <c r="AH22" s="0" t="n">
+      <c r="AH22" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="AI22" s="0" t="n">
+      <c r="AI22" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="AJ22" s="0" t="n">
+      <c r="AJ22" s="1" t="n">
         <v>3.92</v>
       </c>
     </row>
@@ -3170,13 +3170,13 @@
       <c r="AF23" s="2" t="n">
         <v>1.96026490066225</v>
       </c>
-      <c r="AH23" s="0" t="n">
+      <c r="AH23" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI23" s="0" t="n">
+      <c r="AI23" s="1" t="n">
         <v>-0.53</v>
       </c>
-      <c r="AJ23" s="0" t="n">
+      <c r="AJ23" s="1" t="n">
         <v>-0.3</v>
       </c>
     </row>
@@ -3277,13 +3277,13 @@
       <c r="AF24" s="2" t="n">
         <v>-0.95364238410596</v>
       </c>
-      <c r="AH24" s="0" t="n">
+      <c r="AH24" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI24" s="0" t="n">
+      <c r="AI24" s="1" t="n">
         <v>3.68</v>
       </c>
-      <c r="AJ24" s="0" t="n">
+      <c r="AJ24" s="1" t="n">
         <v>9.38</v>
       </c>
     </row>
@@ -3384,13 +3384,13 @@
       <c r="AF25" s="2" t="n">
         <v>6.06622516556291</v>
       </c>
-      <c r="AH25" s="0" t="n">
+      <c r="AH25" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="AI25" s="0" t="n">
+      <c r="AI25" s="1" t="n">
         <v>1.06</v>
       </c>
-      <c r="AJ25" s="0" t="n">
+      <c r="AJ25" s="1" t="n">
         <v>0.76</v>
       </c>
     </row>
@@ -3491,13 +3491,13 @@
       <c r="AF26" s="2" t="n">
         <v>4.60927152317881</v>
       </c>
-      <c r="AH26" s="0" t="n">
+      <c r="AH26" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI26" s="0" t="n">
+      <c r="AI26" s="1" t="n">
         <v>1.9</v>
       </c>
-      <c r="AJ26" s="0" t="n">
+      <c r="AJ26" s="1" t="n">
         <v>2.32</v>
       </c>
     </row>
@@ -3598,13 +3598,13 @@
       <c r="AF27" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
-      <c r="AH27" s="0" t="n">
+      <c r="AH27" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="AI27" s="0" t="n">
+      <c r="AI27" s="1" t="n">
         <v>-1.37</v>
       </c>
-      <c r="AJ27" s="0" t="n">
+      <c r="AJ27" s="1" t="n">
         <v>-1.85</v>
       </c>
     </row>
@@ -3705,13 +3705,13 @@
       <c r="AF28" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
-      <c r="AH28" s="0" t="n">
+      <c r="AH28" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI28" s="0" t="n">
+      <c r="AI28" s="1" t="n">
         <v>1.9</v>
       </c>
-      <c r="AJ28" s="0" t="n">
+      <c r="AJ28" s="1" t="n">
         <v>4.35</v>
       </c>
     </row>
@@ -3812,13 +3812,13 @@
       <c r="AF29" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
-      <c r="AH29" s="0" t="n">
+      <c r="AH29" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="AI29" s="0" t="n">
+      <c r="AI29" s="1" t="n">
         <v>-0.52</v>
       </c>
-      <c r="AJ29" s="0" t="n">
+      <c r="AJ29" s="1" t="n">
         <v>-1.15</v>
       </c>
     </row>
@@ -3919,13 +3919,13 @@
       <c r="AF30" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
-      <c r="AH30" s="0" t="n">
+      <c r="AH30" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI30" s="0" t="n">
+      <c r="AI30" s="1" t="n">
         <v>1.93</v>
       </c>
-      <c r="AJ30" s="0" t="n">
+      <c r="AJ30" s="1" t="n">
         <v>4.83</v>
       </c>
     </row>
@@ -4026,13 +4026,13 @@
       <c r="AF31" s="2" t="n">
         <v>3.94701986754967</v>
       </c>
-      <c r="AH31" s="0" t="n">
+      <c r="AH31" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI31" s="0" t="n">
+      <c r="AI31" s="1" t="n">
         <v>0.76</v>
       </c>
-      <c r="AJ31" s="0" t="n">
+      <c r="AJ31" s="1" t="n">
         <v>1.36</v>
       </c>
     </row>
@@ -4133,13 +4133,13 @@
       <c r="AF32" s="2" t="n">
         <v>3.90232558139535</v>
       </c>
-      <c r="AH32" s="0" t="n">
+      <c r="AH32" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI32" s="0" t="n">
+      <c r="AI32" s="1" t="n">
         <v>-1.49</v>
       </c>
-      <c r="AJ32" s="0" t="n">
+      <c r="AJ32" s="1" t="n">
         <v>-1.53</v>
       </c>
     </row>
@@ -4240,13 +4240,13 @@
       <c r="AF33" s="2" t="n">
         <v>0.87906976744186</v>
       </c>
-      <c r="AH33" s="0" t="n">
+      <c r="AH33" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="AI33" s="0" t="n">
+      <c r="AI33" s="1" t="n">
         <v>-0.63</v>
       </c>
-      <c r="AJ33" s="0" t="n">
+      <c r="AJ33" s="1" t="n">
         <v>-1.94</v>
       </c>
     </row>
@@ -4347,13 +4347,13 @@
       <c r="AF34" s="2" t="n">
         <v>2.04186046511628</v>
       </c>
-      <c r="AH34" s="0" t="n">
+      <c r="AH34" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI34" s="0" t="n">
+      <c r="AI34" s="1" t="n">
         <v>-0.84</v>
       </c>
-      <c r="AJ34" s="0" t="n">
+      <c r="AJ34" s="1" t="n">
         <v>-1.46</v>
       </c>
     </row>
@@ -4454,13 +4454,13 @@
       <c r="AF35" s="2" t="n">
         <v>0.995348837209302</v>
       </c>
-      <c r="AH35" s="0" t="n">
+      <c r="AH35" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI35" s="0" t="n">
+      <c r="AI35" s="1" t="n">
         <v>-1.02</v>
       </c>
-      <c r="AJ35" s="0" t="n">
+      <c r="AJ35" s="1" t="n">
         <v>-1.19</v>
       </c>
     </row>
@@ -4561,13 +4561,13 @@
       <c r="AF36" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
-      <c r="AH36" s="0" t="n">
+      <c r="AH36" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="AI36" s="0" t="n">
+      <c r="AI36" s="1" t="n">
         <v>-0.66</v>
       </c>
-      <c r="AJ36" s="0" t="n">
+      <c r="AJ36" s="1" t="n">
         <v>-0.47</v>
       </c>
     </row>
@@ -4668,13 +4668,13 @@
       <c r="AF37" s="2" t="n">
         <v>12.7395348837209</v>
       </c>
-      <c r="AH37" s="0" t="n">
+      <c r="AH37" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI37" s="0" t="n">
+      <c r="AI37" s="1" t="n">
         <v>1.07</v>
       </c>
-      <c r="AJ37" s="0" t="n">
+      <c r="AJ37" s="1" t="n">
         <v>0.89</v>
       </c>
     </row>
@@ -4775,13 +4775,13 @@
       <c r="AF38" s="2" t="n">
         <v>-0.0511627906976746</v>
       </c>
-      <c r="AH38" s="0" t="n">
+      <c r="AH38" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="AI38" s="0" t="n">
+      <c r="AI38" s="1" t="n">
         <v>1.56</v>
       </c>
-      <c r="AJ38" s="0" t="n">
+      <c r="AJ38" s="1" t="n">
         <v>3.73</v>
       </c>
     </row>
@@ -4882,13 +4882,13 @@
       <c r="AF39" s="2" t="n">
         <v>0.181395348837209</v>
       </c>
-      <c r="AH39" s="0" t="n">
+      <c r="AH39" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="AI39" s="0" t="n">
+      <c r="AI39" s="1" t="n">
         <v>-1.67</v>
       </c>
-      <c r="AJ39" s="0" t="n">
+      <c r="AJ39" s="1" t="n">
         <v>-1.85</v>
       </c>
     </row>
@@ -4989,13 +4989,13 @@
       <c r="AF40" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
-      <c r="AH40" s="0" t="n">
+      <c r="AH40" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="AI40" s="0" t="n">
+      <c r="AI40" s="1" t="n">
         <v>-0.56</v>
       </c>
-      <c r="AJ40" s="0" t="n">
+      <c r="AJ40" s="1" t="n">
         <v>-0.13</v>
       </c>
     </row>
@@ -5096,13 +5096,13 @@
       <c r="AF41" s="2" t="n">
         <v>4.01860465116279</v>
       </c>
-      <c r="AH41" s="0" t="n">
+      <c r="AH41" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AI41" s="0" t="n">
+      <c r="AI41" s="1" t="n">
         <v>-0.05</v>
       </c>
-      <c r="AJ41" s="0" t="n">
+      <c r="AJ41" s="1" t="n">
         <v>1.39</v>
       </c>
     </row>
@@ -5203,13 +5203,13 @@
       <c r="AF42" s="2" t="n">
         <v>5.64651162790698</v>
       </c>
-      <c r="AH42" s="0" t="n">
+      <c r="AH42" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="AI42" s="0" t="n">
+      <c r="AI42" s="1" t="n">
         <v>1.27</v>
       </c>
-      <c r="AJ42" s="0" t="n">
+      <c r="AJ42" s="1" t="n">
         <v>2.9</v>
       </c>
     </row>
@@ -5310,13 +5310,13 @@
       <c r="AF43" s="2" t="n">
         <v>-0.0264900662251655</v>
       </c>
-      <c r="AH43" s="0" t="n">
+      <c r="AH43" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="AI43" s="0" t="n">
+      <c r="AI43" s="1" t="n">
         <v>-0.81</v>
       </c>
-      <c r="AJ43" s="0" t="n">
+      <c r="AJ43" s="1" t="n">
         <v>-0.26</v>
       </c>
     </row>
@@ -5417,13 +5417,13 @@
       <c r="AF44" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
-      <c r="AH44" s="0" t="n">
+      <c r="AH44" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="AI44" s="0" t="n">
+      <c r="AI44" s="1" t="n">
         <v>1.11</v>
       </c>
-      <c r="AJ44" s="0" t="n">
+      <c r="AJ44" s="1" t="n">
         <v>7.15</v>
       </c>
     </row>
@@ -5524,13 +5524,13 @@
       <c r="AF45" s="2" t="n">
         <v>3.68211920529801</v>
       </c>
-      <c r="AH45" s="0" t="n">
+      <c r="AH45" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI45" s="0" t="n">
+      <c r="AI45" s="1" t="n">
         <v>0.78</v>
       </c>
-      <c r="AJ45" s="0" t="n">
+      <c r="AJ45" s="1" t="n">
         <v>0.16</v>
       </c>
     </row>
@@ -5631,13 +5631,13 @@
       <c r="AF46" s="2" t="n">
         <v>1.82781456953642</v>
       </c>
-      <c r="AH46" s="0" t="n">
+      <c r="AH46" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI46" s="0" t="n">
+      <c r="AI46" s="1" t="n">
         <v>0.49</v>
       </c>
-      <c r="AJ46" s="0" t="n">
+      <c r="AJ46" s="1" t="n">
         <v>2.79</v>
       </c>
     </row>
@@ -5738,13 +5738,13 @@
       <c r="AF47" s="2" t="n">
         <v>0.370860927152318</v>
       </c>
-      <c r="AH47" s="0" t="n">
+      <c r="AH47" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="AI47" s="0" t="n">
+      <c r="AI47" s="1" t="n">
         <v>-0.76</v>
       </c>
-      <c r="AJ47" s="0" t="n">
+      <c r="AJ47" s="1" t="n">
         <v>-1.13</v>
       </c>
     </row>
@@ -5845,13 +5845,13 @@
       <c r="AF48" s="2" t="n">
         <v>3.1523178807947</v>
       </c>
-      <c r="AH48" s="0" t="n">
+      <c r="AH48" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="AI48" s="0" t="n">
+      <c r="AI48" s="1" t="n">
         <v>9.32</v>
       </c>
-      <c r="AJ48" s="0" t="n">
+      <c r="AJ48" s="1" t="n">
         <v>49.97</v>
       </c>
     </row>
@@ -5952,13 +5952,13 @@
       <c r="AF49" s="2" t="n">
         <v>2.35761589403974</v>
       </c>
-      <c r="AH49" s="0" t="n">
+      <c r="AH49" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AI49" s="0" t="n">
+      <c r="AI49" s="1" t="n">
         <v>-0.06</v>
       </c>
-      <c r="AJ49" s="0" t="n">
+      <c r="AJ49" s="1" t="n">
         <v>-0.03</v>
       </c>
     </row>
@@ -6059,13 +6059,13 @@
       <c r="AF50" s="2" t="n">
         <v>5.00662251655629</v>
       </c>
-      <c r="AH50" s="0" t="n">
+      <c r="AH50" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI50" s="0" t="n">
+      <c r="AI50" s="1" t="n">
         <v>-0.9</v>
       </c>
-      <c r="AJ50" s="0" t="n">
+      <c r="AJ50" s="1" t="n">
         <v>-1.7</v>
       </c>
     </row>
@@ -6166,13 +6166,13 @@
       <c r="AF51" s="2" t="n">
         <v>0.900662251655629</v>
       </c>
-      <c r="AH51" s="0" t="n">
+      <c r="AH51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI51" s="0" t="n">
+      <c r="AI51" s="1" t="n">
         <v>1.05</v>
       </c>
-      <c r="AJ51" s="0" t="n">
+      <c r="AJ51" s="1" t="n">
         <v>4.98</v>
       </c>
     </row>
@@ -6273,13 +6273,13 @@
       <c r="AF52" s="2" t="n">
         <v>4.0794701986755</v>
       </c>
-      <c r="AH52" s="0" t="n">
+      <c r="AH52" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="AI52" s="0" t="n">
+      <c r="AI52" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="AJ52" s="0" t="n">
+      <c r="AJ52" s="1" t="n">
         <v>0.68</v>
       </c>
     </row>
@@ -6380,13 +6380,13 @@
       <c r="AF53" s="2" t="n">
         <v>-0.291390728476821</v>
       </c>
-      <c r="AH53" s="0" t="n">
+      <c r="AH53" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI53" s="0" t="n">
+      <c r="AI53" s="1" t="n">
         <v>4.16</v>
       </c>
-      <c r="AJ53" s="0" t="n">
+      <c r="AJ53" s="1" t="n">
         <v>20.55</v>
       </c>
     </row>
@@ -6487,13 +6487,13 @@
       <c r="AF54" s="2" t="n">
         <v>2.88741721854305</v>
       </c>
-      <c r="AH54" s="0" t="n">
+      <c r="AH54" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="AI54" s="0" t="n">
+      <c r="AI54" s="1" t="n">
         <v>-0.64</v>
       </c>
-      <c r="AJ54" s="0" t="n">
+      <c r="AJ54" s="1" t="n">
         <v>-0.36</v>
       </c>
     </row>
@@ -6594,13 +6594,13 @@
       <c r="AF55" s="2" t="n">
         <v>6.19867549668874</v>
       </c>
-      <c r="AH55" s="0" t="n">
+      <c r="AH55" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI55" s="0" t="n">
+      <c r="AI55" s="1" t="n">
         <v>3.51</v>
       </c>
-      <c r="AJ55" s="0" t="n">
+      <c r="AJ55" s="1" t="n">
         <v>29.48</v>
       </c>
     </row>
@@ -6701,13 +6701,13 @@
       <c r="AF56" s="2" t="n">
         <v>-1.74834437086093</v>
       </c>
-      <c r="AH56" s="0" t="n">
+      <c r="AH56" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="AI56" s="0" t="n">
+      <c r="AI56" s="1" t="n">
         <v>0.29</v>
       </c>
-      <c r="AJ56" s="0" t="n">
+      <c r="AJ56" s="1" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -6808,13 +6808,13 @@
       <c r="AF57" s="2" t="n">
         <v>0.503311258278146</v>
       </c>
-      <c r="AH57" s="0" t="n">
+      <c r="AH57" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI57" s="0" t="n">
+      <c r="AI57" s="1" t="n">
         <v>-0.78</v>
       </c>
-      <c r="AJ57" s="0" t="n">
+      <c r="AJ57" s="1" t="n">
         <v>-1.36</v>
       </c>
     </row>
@@ -6915,13 +6915,13 @@
       <c r="AF58" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
-      <c r="AH58" s="0" t="n">
+      <c r="AH58" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="AI58" s="0" t="n">
+      <c r="AI58" s="1" t="n">
         <v>-0.59</v>
       </c>
-      <c r="AJ58" s="0" t="n">
+      <c r="AJ58" s="1" t="n">
         <v>0.18</v>
       </c>
     </row>
@@ -7022,13 +7022,13 @@
       <c r="AF59" s="2" t="n">
         <v>2.62251655629139</v>
       </c>
-      <c r="AH59" s="0" t="n">
+      <c r="AH59" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="AI59" s="0" t="n">
+      <c r="AI59" s="1" t="n">
         <v>999</v>
       </c>
-      <c r="AJ59" s="0" t="n">
+      <c r="AJ59" s="1" t="n">
         <v>999</v>
       </c>
     </row>
@@ -7129,13 +7129,13 @@
       <c r="AF60" s="2" t="n">
         <v>3.81456953642384</v>
       </c>
-      <c r="AH60" s="0" t="n">
+      <c r="AH60" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI60" s="0" t="n">
+      <c r="AI60" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="AJ60" s="0" t="n">
+      <c r="AJ60" s="1" t="n">
         <v>0.68</v>
       </c>
     </row>
@@ -7236,13 +7236,13 @@
       <c r="AF61" s="2" t="n">
         <v>1.82781456953642</v>
       </c>
-      <c r="AH61" s="0" t="n">
+      <c r="AH61" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="AI61" s="0" t="n">
+      <c r="AI61" s="1" t="n">
         <v>0.59</v>
       </c>
-      <c r="AJ61" s="0" t="n">
+      <c r="AJ61" s="1" t="n">
         <v>2.14</v>
       </c>
     </row>
@@ -7343,13 +7343,13 @@
       <c r="AF62" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
-      <c r="AH62" s="0" t="n">
+      <c r="AH62" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="AI62" s="0" t="n">
+      <c r="AI62" s="1" t="n">
         <v>0.46</v>
       </c>
-      <c r="AJ62" s="0" t="n">
+      <c r="AJ62" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7450,13 +7450,13 @@
       <c r="AF63" s="2" t="n">
         <v>1.43046357615894</v>
       </c>
-      <c r="AH63" s="0" t="n">
+      <c r="AH63" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI63" s="0" t="n">
+      <c r="AI63" s="1" t="n">
         <v>-1.46</v>
       </c>
-      <c r="AJ63" s="0" t="n">
+      <c r="AJ63" s="1" t="n">
         <v>-2.62</v>
       </c>
     </row>
@@ -7557,13 +7557,13 @@
       <c r="AF64" s="2" t="n">
         <v>0.635761589403974</v>
       </c>
-      <c r="AH64" s="0" t="n">
+      <c r="AH64" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="AI64" s="0" t="n">
+      <c r="AI64" s="1" t="n">
         <v>5.88</v>
       </c>
-      <c r="AJ64" s="0" t="n">
+      <c r="AJ64" s="1" t="n">
         <v>49.97</v>
       </c>
     </row>
@@ -7664,13 +7664,13 @@
       <c r="AF65" s="2" t="n">
         <v>3.01986754966887</v>
       </c>
-      <c r="AH65" s="0" t="n">
+      <c r="AH65" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="AI65" s="0" t="n">
+      <c r="AI65" s="1" t="n">
         <v>-0.05</v>
       </c>
-      <c r="AJ65" s="0" t="n">
+      <c r="AJ65" s="1" t="n">
         <v>1.78</v>
       </c>
     </row>
@@ -7771,13 +7771,13 @@
       <c r="AF66" s="2" t="n">
         <v>4.25116279069768</v>
       </c>
-      <c r="AH66" s="0" t="n">
+      <c r="AH66" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI66" s="0" t="n">
+      <c r="AI66" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="AJ66" s="0" t="n">
+      <c r="AJ66" s="1" t="n">
         <v>1.02</v>
       </c>
     </row>
@@ -7878,13 +7878,13 @@
       <c r="AF67" s="2" t="n">
         <v>-0.167441860465116</v>
       </c>
-      <c r="AH67" s="0" t="n">
+      <c r="AH67" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI67" s="0" t="n">
+      <c r="AI67" s="1" t="n">
         <v>-0.05</v>
       </c>
-      <c r="AJ67" s="0" t="n">
+      <c r="AJ67" s="1" t="n">
         <v>-0.36</v>
       </c>
     </row>
@@ -7985,13 +7985,13 @@
       <c r="AF68" s="2" t="n">
         <v>2.73953488372093</v>
       </c>
-      <c r="AH68" s="0" t="n">
+      <c r="AH68" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="AI68" s="0" t="n">
+      <c r="AI68" s="1" t="n">
         <v>2.49</v>
       </c>
-      <c r="AJ68" s="0" t="n">
+      <c r="AJ68" s="1" t="n">
         <v>8.24</v>
       </c>
     </row>
@@ -8092,13 +8092,13 @@
       <c r="AF69" s="2" t="n">
         <v>-1.33023255813954</v>
       </c>
-      <c r="AH69" s="0" t="n">
+      <c r="AH69" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI69" s="0" t="n">
+      <c r="AI69" s="1" t="n">
         <v>1.78</v>
       </c>
-      <c r="AJ69" s="0" t="n">
+      <c r="AJ69" s="1" t="n">
         <v>5.02</v>
       </c>
     </row>
@@ -8199,13 +8199,13 @@
       <c r="AF70" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
-      <c r="AH70" s="0" t="n">
+      <c r="AH70" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="AI70" s="0" t="n">
+      <c r="AI70" s="1" t="n">
         <v>-0.22</v>
       </c>
-      <c r="AJ70" s="0" t="n">
+      <c r="AJ70" s="1" t="n">
         <v>-0.23</v>
       </c>
     </row>
@@ -8306,13 +8306,13 @@
       <c r="AF71" s="2" t="n">
         <v>-0.516279069767442</v>
       </c>
-      <c r="AH71" s="0" t="n">
+      <c r="AH71" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI71" s="0" t="n">
+      <c r="AI71" s="1" t="n">
         <v>-0.39</v>
       </c>
-      <c r="AJ71" s="0" t="n">
+      <c r="AJ71" s="1" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -8413,13 +8413,13 @@
       <c r="AF72" s="2" t="n">
         <v>2.97209302325581</v>
       </c>
-      <c r="AH72" s="0" t="n">
+      <c r="AH72" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI72" s="0" t="n">
+      <c r="AI72" s="1" t="n">
         <v>-1.07</v>
       </c>
-      <c r="AJ72" s="0" t="n">
+      <c r="AJ72" s="1" t="n">
         <v>-0.85</v>
       </c>
     </row>
@@ -8520,13 +8520,13 @@
       <c r="AF73" s="2" t="n">
         <v>3.32093023255814</v>
       </c>
-      <c r="AH73" s="0" t="n">
+      <c r="AH73" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="AI73" s="0" t="n">
+      <c r="AI73" s="1" t="n">
         <v>-0.95</v>
       </c>
-      <c r="AJ73" s="0" t="n">
+      <c r="AJ73" s="1" t="n">
         <v>-0.32</v>
       </c>
     </row>
@@ -8627,13 +8627,13 @@
       <c r="AF74" s="2" t="n">
         <v>2.39069767441861</v>
       </c>
-      <c r="AH74" s="0" t="n">
+      <c r="AH74" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="AI74" s="0" t="n">
+      <c r="AI74" s="1" t="n">
         <v>0.37</v>
       </c>
-      <c r="AJ74" s="0" t="n">
+      <c r="AJ74" s="1" t="n">
         <v>0.13</v>
       </c>
     </row>
@@ -8734,13 +8734,13 @@
       <c r="AF75" s="2" t="n">
         <v>4.48372093023256</v>
       </c>
-      <c r="AH75" s="0" t="n">
+      <c r="AH75" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="AI75" s="0" t="n">
+      <c r="AI75" s="1" t="n">
         <v>-1.24</v>
       </c>
-      <c r="AJ75" s="0" t="n">
+      <c r="AJ75" s="1" t="n">
         <v>-1.04</v>
       </c>
     </row>
@@ -8841,13 +8841,13 @@
       <c r="AF76" s="2" t="n">
         <v>-0.0511627906976746</v>
       </c>
-      <c r="AH76" s="0" t="n">
+      <c r="AH76" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="AI76" s="0" t="n">
+      <c r="AI76" s="1" t="n">
         <v>1.04</v>
       </c>
-      <c r="AJ76" s="0" t="n">
+      <c r="AJ76" s="1" t="n">
         <v>3.4</v>
       </c>
     </row>
@@ -8948,13 +8948,13 @@
       <c r="AF77" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
-      <c r="AH77" s="0" t="n">
+      <c r="AH77" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="AI77" s="0" t="n">
+      <c r="AI77" s="1" t="n">
         <v>-0.47</v>
       </c>
-      <c r="AJ77" s="0" t="n">
+      <c r="AJ77" s="1" t="n">
         <v>2.76</v>
       </c>
     </row>
@@ -9055,13 +9055,13 @@
       <c r="AF78" s="2" t="n">
         <v>999</v>
       </c>
-      <c r="AH78" s="0" t="n">
+      <c r="AH78" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="AI78" s="0" t="n">
+      <c r="AI78" s="1" t="n">
         <v>0.23</v>
       </c>
-      <c r="AJ78" s="0" t="n">
+      <c r="AJ78" s="1" t="n">
         <v>1.27</v>
       </c>
     </row>
@@ -9162,13 +9162,13 @@
       <c r="AF79" s="2" t="n">
         <v>-0.4</v>
       </c>
-      <c r="AH79" s="0" t="n">
+      <c r="AH79" s="1" t="n">
         <v>999</v>
       </c>
-      <c r="AI79" s="0" t="n">
+      <c r="AI79" s="1" t="n">
         <v>999</v>
       </c>
-      <c r="AJ79" s="0" t="n">
+      <c r="AJ79" s="1" t="n">
         <v>999</v>
       </c>
     </row>
@@ -9269,13 +9269,13 @@
       <c r="AF80" s="2" t="n">
         <v>-1.67906976744186</v>
       </c>
-      <c r="AH80" s="0" t="n">
+      <c r="AH80" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="AI80" s="0" t="n">
+      <c r="AI80" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="AJ80" s="0" t="n">
+      <c r="AJ80" s="1" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -9376,13 +9376,13 @@
       <c r="AF81" s="2" t="n">
         <v>2.38156359393232</v>
       </c>
-      <c r="AH81" s="0" t="n">
+      <c r="AH81" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="AI81" s="0" t="n">
+      <c r="AI81" s="1" t="n">
         <v>1.42</v>
       </c>
-      <c r="AJ81" s="0" t="n">
+      <c r="AJ81" s="1" t="n">
         <v>3.14</v>
       </c>
     </row>
@@ -9483,13 +9483,13 @@
       <c r="AF82" s="2" t="n">
         <v>-0.283720930232558</v>
       </c>
-      <c r="AH82" s="0" t="n">
+      <c r="AH82" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="AI82" s="0" t="n">
+      <c r="AI82" s="1" t="n">
         <v>-0.06</v>
       </c>
-      <c r="AJ82" s="0" t="n">
+      <c r="AJ82" s="1" t="n">
         <v>-0.19</v>
       </c>
     </row>
@@ -9506,7 +9506,7 @@
       <c r="D83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E83" s="3" t="n">
+      <c r="E83" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F83" s="2" t="n">
@@ -9590,13 +9590,13 @@
       <c r="AF83" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
-      <c r="AH83" s="0" t="n">
+      <c r="AH83" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="AI83" s="0" t="n">
+      <c r="AI83" s="1" t="n">
         <v>1.07</v>
       </c>
-      <c r="AJ83" s="0" t="n">
+      <c r="AJ83" s="1" t="n">
         <v>1.69</v>
       </c>
     </row>
@@ -9613,7 +9613,7 @@
       <c r="D84" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E84" s="3" t="n">
+      <c r="E84" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F84" s="2" t="n">
@@ -12050,8 +12050,14 @@
         <v>0.646511627906977</v>
       </c>
     </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E112" s="1" t="n">
+        <f aca="false">E107+E80</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E3 E85:E108">
+  <conditionalFormatting sqref="E1:E3">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>2</formula>
     </cfRule>
@@ -12111,7 +12117,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82:E84">
+  <conditionalFormatting sqref="E82">
     <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>2</formula>
     </cfRule>

</xml_diff>

<commit_message>
change 999 to means, histograms
</commit_message>
<xml_diff>
--- a/data/ADHD_MC.xlsx
+++ b/data/ADHD_MC.xlsx
@@ -708,15 +708,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ112"/>
+  <dimension ref="A1:AI108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,13 +817,13 @@
       <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="AH1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -923,13 +924,13 @@
       <c r="AF2" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
+      <c r="AG2" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH2" s="1" t="n">
-        <v>51</v>
+        <v>1.19</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
         <v>4.67</v>
       </c>
     </row>
@@ -1030,13 +1031,13 @@
       <c r="AF3" s="2" t="n">
         <v>-0.0264900662251655</v>
       </c>
+      <c r="AG3" s="1" t="n">
+        <v>54</v>
+      </c>
       <c r="AH3" s="1" t="n">
-        <v>54</v>
+        <v>-0.84</v>
       </c>
       <c r="AI3" s="1" t="n">
-        <v>-0.84</v>
-      </c>
-      <c r="AJ3" s="1" t="n">
         <v>-1.46</v>
       </c>
     </row>
@@ -1137,13 +1138,13 @@
       <c r="AF4" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
+      <c r="AG4" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH4" s="1" t="n">
-        <v>51</v>
+        <v>1.31</v>
       </c>
       <c r="AI4" s="1" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="AJ4" s="1" t="n">
         <v>1.91</v>
       </c>
     </row>
@@ -1244,13 +1245,13 @@
       <c r="AF5" s="2" t="n">
         <v>3.41721854304636</v>
       </c>
+      <c r="AG5" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="AH5" s="1" t="n">
-        <v>48</v>
+        <v>-0.4</v>
       </c>
       <c r="AI5" s="1" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="AJ5" s="1" t="n">
         <v>-1.27</v>
       </c>
     </row>
@@ -1351,13 +1352,13 @@
       <c r="AF6" s="2" t="n">
         <v>2.62251655629139</v>
       </c>
+      <c r="AG6" s="1" t="n">
+        <v>55</v>
+      </c>
       <c r="AH6" s="1" t="n">
-        <v>55</v>
+        <v>-1.49</v>
       </c>
       <c r="AI6" s="1" t="n">
-        <v>-1.49</v>
-      </c>
-      <c r="AJ6" s="1" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -1458,13 +1459,13 @@
       <c r="AF7" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
+      <c r="AG7" s="1" t="n">
+        <v>42</v>
+      </c>
       <c r="AH7" s="1" t="n">
-        <v>42</v>
+        <v>2.32</v>
       </c>
       <c r="AI7" s="1" t="n">
-        <v>2.32</v>
-      </c>
-      <c r="AJ7" s="1" t="n">
         <v>1.93</v>
       </c>
     </row>
@@ -1565,13 +1566,13 @@
       <c r="AF8" s="2" t="n">
         <v>3.1523178807947</v>
       </c>
+      <c r="AG8" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH8" s="1" t="n">
-        <v>47</v>
+        <v>1.93</v>
       </c>
       <c r="AI8" s="1" t="n">
-        <v>1.93</v>
-      </c>
-      <c r="AJ8" s="1" t="n">
         <v>4.95</v>
       </c>
     </row>
@@ -1672,13 +1673,13 @@
       <c r="AF9" s="2" t="n">
         <v>3.81456953642384</v>
       </c>
+      <c r="AG9" s="1" t="n">
+        <v>54</v>
+      </c>
       <c r="AH9" s="1" t="n">
-        <v>54</v>
+        <v>0.88</v>
       </c>
       <c r="AI9" s="1" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="AJ9" s="1" t="n">
         <v>3.92</v>
       </c>
     </row>
@@ -1779,13 +1780,13 @@
       <c r="AF10" s="2" t="n">
         <v>1.43046357615894</v>
       </c>
+      <c r="AG10" s="1" t="n">
+        <v>58</v>
+      </c>
       <c r="AH10" s="1" t="n">
-        <v>58</v>
+        <v>-1.31</v>
       </c>
       <c r="AI10" s="1" t="n">
-        <v>-1.31</v>
-      </c>
-      <c r="AJ10" s="1" t="n">
         <v>0.18</v>
       </c>
     </row>
@@ -1886,13 +1887,13 @@
       <c r="AF11" s="2" t="n">
         <v>1.03311258278146</v>
       </c>
+      <c r="AG11" s="1" t="n">
+        <v>53</v>
+      </c>
       <c r="AH11" s="1" t="n">
-        <v>53</v>
+        <v>-1.24</v>
       </c>
       <c r="AI11" s="1" t="n">
-        <v>-1.24</v>
-      </c>
-      <c r="AJ11" s="1" t="n">
         <v>-0.88</v>
       </c>
     </row>
@@ -1993,13 +1994,13 @@
       <c r="AF12" s="2" t="n">
         <v>3.01986754966887</v>
       </c>
+      <c r="AG12" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH12" s="1" t="n">
-        <v>50</v>
+        <v>0.45</v>
       </c>
       <c r="AI12" s="1" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="AJ12" s="1" t="n">
         <v>2.25</v>
       </c>
     </row>
@@ -2100,13 +2101,13 @@
       <c r="AF13" s="2" t="n">
         <v>1.56291390728477</v>
       </c>
+      <c r="AG13" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH13" s="1" t="n">
-        <v>47</v>
+        <v>2.24</v>
       </c>
       <c r="AI13" s="1" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="AJ13" s="1" t="n">
         <v>3.11</v>
       </c>
     </row>
@@ -2207,13 +2208,13 @@
       <c r="AF14" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
+      <c r="AG14" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH14" s="1" t="n">
-        <v>49</v>
+        <v>-1.15</v>
       </c>
       <c r="AI14" s="1" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="AJ14" s="1" t="n">
         <v>-0.39</v>
       </c>
     </row>
@@ -2314,13 +2315,13 @@
       <c r="AF15" s="2" t="n">
         <v>2.35761589403974</v>
       </c>
+      <c r="AG15" s="1" t="n">
+        <v>45</v>
+      </c>
       <c r="AH15" s="1" t="n">
-        <v>45</v>
+        <v>2.21</v>
       </c>
       <c r="AI15" s="1" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="AJ15" s="1" t="n">
         <v>4.89</v>
       </c>
     </row>
@@ -2421,13 +2422,13 @@
       <c r="AF16" s="2" t="n">
         <v>3.41721854304636</v>
       </c>
+      <c r="AG16" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH16" s="1" t="n">
-        <v>52</v>
+        <v>-0.73</v>
       </c>
       <c r="AI16" s="1" t="n">
-        <v>-0.73</v>
-      </c>
-      <c r="AJ16" s="1" t="n">
         <v>-0.88</v>
       </c>
     </row>
@@ -2528,13 +2529,13 @@
       <c r="AF17" s="2" t="n">
         <v>1.03311258278146</v>
       </c>
+      <c r="AG17" s="1" t="n">
+        <v>41</v>
+      </c>
       <c r="AH17" s="1" t="n">
-        <v>41</v>
+        <v>2.32</v>
       </c>
       <c r="AI17" s="1" t="n">
-        <v>2.32</v>
-      </c>
-      <c r="AJ17" s="1" t="n">
         <v>2.63</v>
       </c>
     </row>
@@ -2635,13 +2636,13 @@
       <c r="AF18" s="2" t="n">
         <v>0.768211920529802</v>
       </c>
+      <c r="AG18" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH18" s="1" t="n">
-        <v>52</v>
+        <v>-0.81</v>
       </c>
       <c r="AI18" s="1" t="n">
-        <v>-0.81</v>
-      </c>
-      <c r="AJ18" s="1" t="n">
         <v>-0.65</v>
       </c>
     </row>
@@ -2742,13 +2743,13 @@
       <c r="AF19" s="2" t="n">
         <v>1.96026490066225</v>
       </c>
+      <c r="AG19" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH19" s="1" t="n">
-        <v>50</v>
+        <v>0.33</v>
       </c>
       <c r="AI19" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="AJ19" s="1" t="n">
         <v>1.08</v>
       </c>
     </row>
@@ -2849,13 +2850,13 @@
       <c r="AF20" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
+      <c r="AG20" s="1" t="n">
+        <v>53</v>
+      </c>
       <c r="AH20" s="1" t="n">
-        <v>53</v>
+        <v>-0.06</v>
       </c>
       <c r="AI20" s="1" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="AJ20" s="1" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -2956,13 +2957,13 @@
       <c r="AF21" s="2" t="n">
         <v>1.6953642384106</v>
       </c>
+      <c r="AG21" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH21" s="1" t="n">
-        <v>52</v>
+        <v>0.41</v>
       </c>
       <c r="AI21" s="1" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="AJ21" s="1" t="n">
         <v>3.84</v>
       </c>
     </row>
@@ -3063,13 +3064,13 @@
       <c r="AF22" s="2" t="n">
         <v>4.34437086092715</v>
       </c>
+      <c r="AG22" s="1" t="n">
+        <v>46</v>
+      </c>
       <c r="AH22" s="1" t="n">
-        <v>46</v>
+        <v>1.71</v>
       </c>
       <c r="AI22" s="1" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="AJ22" s="1" t="n">
         <v>3.92</v>
       </c>
     </row>
@@ -3170,13 +3171,13 @@
       <c r="AF23" s="2" t="n">
         <v>1.96026490066225</v>
       </c>
+      <c r="AG23" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH23" s="1" t="n">
-        <v>52</v>
+        <v>-0.53</v>
       </c>
       <c r="AI23" s="1" t="n">
-        <v>-0.53</v>
-      </c>
-      <c r="AJ23" s="1" t="n">
         <v>-0.3</v>
       </c>
     </row>
@@ -3277,13 +3278,13 @@
       <c r="AF24" s="2" t="n">
         <v>-0.95364238410596</v>
       </c>
+      <c r="AG24" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH24" s="1" t="n">
-        <v>49</v>
+        <v>3.68</v>
       </c>
       <c r="AI24" s="1" t="n">
-        <v>3.68</v>
-      </c>
-      <c r="AJ24" s="1" t="n">
         <v>9.38</v>
       </c>
     </row>
@@ -3384,13 +3385,13 @@
       <c r="AF25" s="2" t="n">
         <v>6.06622516556291</v>
       </c>
+      <c r="AG25" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AH25" s="1" t="n">
-        <v>44</v>
+        <v>1.06</v>
       </c>
       <c r="AI25" s="1" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="AJ25" s="1" t="n">
         <v>0.76</v>
       </c>
     </row>
@@ -3491,13 +3492,13 @@
       <c r="AF26" s="2" t="n">
         <v>4.60927152317881</v>
       </c>
+      <c r="AG26" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH26" s="1" t="n">
-        <v>47</v>
+        <v>1.9</v>
       </c>
       <c r="AI26" s="1" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="AJ26" s="1" t="n">
         <v>2.32</v>
       </c>
     </row>
@@ -3598,13 +3599,13 @@
       <c r="AF27" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
+      <c r="AG27" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="AH27" s="1" t="n">
-        <v>59</v>
+        <v>-1.37</v>
       </c>
       <c r="AI27" s="1" t="n">
-        <v>-1.37</v>
-      </c>
-      <c r="AJ27" s="1" t="n">
         <v>-1.85</v>
       </c>
     </row>
@@ -3705,13 +3706,13 @@
       <c r="AF28" s="2" t="n">
         <v>2.09271523178808</v>
       </c>
+      <c r="AG28" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH28" s="1" t="n">
-        <v>47</v>
+        <v>1.9</v>
       </c>
       <c r="AI28" s="1" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="AJ28" s="1" t="n">
         <v>4.35</v>
       </c>
     </row>
@@ -3812,13 +3813,13 @@
       <c r="AF29" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
+      <c r="AG29" s="1" t="n">
+        <v>46</v>
+      </c>
       <c r="AH29" s="1" t="n">
-        <v>46</v>
+        <v>-0.52</v>
       </c>
       <c r="AI29" s="1" t="n">
-        <v>-0.52</v>
-      </c>
-      <c r="AJ29" s="1" t="n">
         <v>-1.15</v>
       </c>
     </row>
@@ -3919,13 +3920,13 @@
       <c r="AF30" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
+      <c r="AG30" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH30" s="1" t="n">
-        <v>49</v>
+        <v>1.93</v>
       </c>
       <c r="AI30" s="1" t="n">
-        <v>1.93</v>
-      </c>
-      <c r="AJ30" s="1" t="n">
         <v>4.83</v>
       </c>
     </row>
@@ -4026,13 +4027,13 @@
       <c r="AF31" s="2" t="n">
         <v>3.94701986754967</v>
       </c>
+      <c r="AG31" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH31" s="1" t="n">
-        <v>47</v>
+        <v>0.76</v>
       </c>
       <c r="AI31" s="1" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="AJ31" s="1" t="n">
         <v>1.36</v>
       </c>
     </row>
@@ -4133,13 +4134,13 @@
       <c r="AF32" s="2" t="n">
         <v>3.90232558139535</v>
       </c>
+      <c r="AG32" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH32" s="1" t="n">
-        <v>47</v>
+        <v>-1.49</v>
       </c>
       <c r="AI32" s="1" t="n">
-        <v>-1.49</v>
-      </c>
-      <c r="AJ32" s="1" t="n">
         <v>-1.53</v>
       </c>
     </row>
@@ -4240,13 +4241,13 @@
       <c r="AF33" s="2" t="n">
         <v>0.87906976744186</v>
       </c>
+      <c r="AG33" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="AH33" s="1" t="n">
-        <v>48</v>
+        <v>-0.63</v>
       </c>
       <c r="AI33" s="1" t="n">
-        <v>-0.63</v>
-      </c>
-      <c r="AJ33" s="1" t="n">
         <v>-1.94</v>
       </c>
     </row>
@@ -4347,13 +4348,13 @@
       <c r="AF34" s="2" t="n">
         <v>2.04186046511628</v>
       </c>
+      <c r="AG34" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH34" s="1" t="n">
-        <v>50</v>
+        <v>-0.84</v>
       </c>
       <c r="AI34" s="1" t="n">
-        <v>-0.84</v>
-      </c>
-      <c r="AJ34" s="1" t="n">
         <v>-1.46</v>
       </c>
     </row>
@@ -4454,13 +4455,13 @@
       <c r="AF35" s="2" t="n">
         <v>0.995348837209302</v>
       </c>
+      <c r="AG35" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH35" s="1" t="n">
-        <v>51</v>
+        <v>-1.02</v>
       </c>
       <c r="AI35" s="1" t="n">
-        <v>-1.02</v>
-      </c>
-      <c r="AJ35" s="1" t="n">
         <v>-1.19</v>
       </c>
     </row>
@@ -4561,13 +4562,13 @@
       <c r="AF36" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
+      <c r="AG36" s="1" t="n">
+        <v>42</v>
+      </c>
       <c r="AH36" s="1" t="n">
-        <v>42</v>
+        <v>-0.66</v>
       </c>
       <c r="AI36" s="1" t="n">
-        <v>-0.66</v>
-      </c>
-      <c r="AJ36" s="1" t="n">
         <v>-0.47</v>
       </c>
     </row>
@@ -4668,13 +4669,13 @@
       <c r="AF37" s="2" t="n">
         <v>12.7395348837209</v>
       </c>
+      <c r="AG37" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH37" s="1" t="n">
-        <v>47</v>
+        <v>1.07</v>
       </c>
       <c r="AI37" s="1" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="AJ37" s="1" t="n">
         <v>0.89</v>
       </c>
     </row>
@@ -4775,13 +4776,13 @@
       <c r="AF38" s="2" t="n">
         <v>-0.0511627906976746</v>
       </c>
+      <c r="AG38" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AH38" s="1" t="n">
-        <v>44</v>
+        <v>1.56</v>
       </c>
       <c r="AI38" s="1" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="AJ38" s="1" t="n">
         <v>3.73</v>
       </c>
     </row>
@@ -4882,13 +4883,13 @@
       <c r="AF39" s="2" t="n">
         <v>0.181395348837209</v>
       </c>
+      <c r="AG39" s="1" t="n">
+        <v>56</v>
+      </c>
       <c r="AH39" s="1" t="n">
-        <v>56</v>
+        <v>-1.67</v>
       </c>
       <c r="AI39" s="1" t="n">
-        <v>-1.67</v>
-      </c>
-      <c r="AJ39" s="1" t="n">
         <v>-1.85</v>
       </c>
     </row>
@@ -4989,13 +4990,13 @@
       <c r="AF40" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
+      <c r="AG40" s="1" t="n">
+        <v>54</v>
+      </c>
       <c r="AH40" s="1" t="n">
-        <v>54</v>
+        <v>-0.56</v>
       </c>
       <c r="AI40" s="1" t="n">
-        <v>-0.56</v>
-      </c>
-      <c r="AJ40" s="1" t="n">
         <v>-0.13</v>
       </c>
     </row>
@@ -5096,13 +5097,13 @@
       <c r="AF41" s="2" t="n">
         <v>4.01860465116279</v>
       </c>
+      <c r="AG41" s="1" t="n">
+        <v>45</v>
+      </c>
       <c r="AH41" s="1" t="n">
-        <v>45</v>
+        <v>-0.05</v>
       </c>
       <c r="AI41" s="1" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="AJ41" s="1" t="n">
         <v>1.39</v>
       </c>
     </row>
@@ -5203,13 +5204,13 @@
       <c r="AF42" s="2" t="n">
         <v>5.64651162790698</v>
       </c>
+      <c r="AG42" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="AH42" s="1" t="n">
-        <v>48</v>
+        <v>1.27</v>
       </c>
       <c r="AI42" s="1" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="AJ42" s="1" t="n">
         <v>2.9</v>
       </c>
     </row>
@@ -5310,13 +5311,13 @@
       <c r="AF43" s="2" t="n">
         <v>-0.0264900662251655</v>
       </c>
+      <c r="AG43" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AH43" s="1" t="n">
-        <v>44</v>
+        <v>-0.81</v>
       </c>
       <c r="AI43" s="1" t="n">
-        <v>-0.81</v>
-      </c>
-      <c r="AJ43" s="1" t="n">
         <v>-0.26</v>
       </c>
     </row>
@@ -5417,13 +5418,13 @@
       <c r="AF44" s="2" t="n">
         <v>1.29801324503311</v>
       </c>
+      <c r="AG44" s="1" t="n">
+        <v>70</v>
+      </c>
       <c r="AH44" s="1" t="n">
-        <v>70</v>
+        <v>1.11</v>
       </c>
       <c r="AI44" s="1" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="AJ44" s="1" t="n">
         <v>7.15</v>
       </c>
     </row>
@@ -5524,13 +5525,13 @@
       <c r="AF45" s="2" t="n">
         <v>3.68211920529801</v>
       </c>
+      <c r="AG45" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH45" s="1" t="n">
-        <v>50</v>
+        <v>0.78</v>
       </c>
       <c r="AI45" s="1" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="AJ45" s="1" t="n">
         <v>0.16</v>
       </c>
     </row>
@@ -5631,13 +5632,13 @@
       <c r="AF46" s="2" t="n">
         <v>1.82781456953642</v>
       </c>
+      <c r="AG46" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH46" s="1" t="n">
-        <v>52</v>
+        <v>0.49</v>
       </c>
       <c r="AI46" s="1" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="AJ46" s="1" t="n">
         <v>2.79</v>
       </c>
     </row>
@@ -5738,13 +5739,13 @@
       <c r="AF47" s="2" t="n">
         <v>0.370860927152318</v>
       </c>
+      <c r="AG47" s="1" t="n">
+        <v>53</v>
+      </c>
       <c r="AH47" s="1" t="n">
-        <v>53</v>
+        <v>-0.76</v>
       </c>
       <c r="AI47" s="1" t="n">
-        <v>-0.76</v>
-      </c>
-      <c r="AJ47" s="1" t="n">
         <v>-1.13</v>
       </c>
     </row>
@@ -5845,13 +5846,13 @@
       <c r="AF48" s="2" t="n">
         <v>3.1523178807947</v>
       </c>
+      <c r="AG48" s="1" t="n">
+        <v>44</v>
+      </c>
       <c r="AH48" s="1" t="n">
-        <v>44</v>
+        <v>9.32</v>
       </c>
       <c r="AI48" s="1" t="n">
-        <v>9.32</v>
-      </c>
-      <c r="AJ48" s="1" t="n">
         <v>49.97</v>
       </c>
     </row>
@@ -5952,13 +5953,13 @@
       <c r="AF49" s="2" t="n">
         <v>2.35761589403974</v>
       </c>
+      <c r="AG49" s="1" t="n">
+        <v>45</v>
+      </c>
       <c r="AH49" s="1" t="n">
-        <v>45</v>
+        <v>-0.06</v>
       </c>
       <c r="AI49" s="1" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="AJ49" s="1" t="n">
         <v>-0.03</v>
       </c>
     </row>
@@ -6059,13 +6060,13 @@
       <c r="AF50" s="2" t="n">
         <v>5.00662251655629</v>
       </c>
+      <c r="AG50" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH50" s="1" t="n">
-        <v>51</v>
+        <v>-0.9</v>
       </c>
       <c r="AI50" s="1" t="n">
-        <v>-0.9</v>
-      </c>
-      <c r="AJ50" s="1" t="n">
         <v>-1.7</v>
       </c>
     </row>
@@ -6166,13 +6167,13 @@
       <c r="AF51" s="2" t="n">
         <v>0.900662251655629</v>
       </c>
+      <c r="AG51" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH51" s="1" t="n">
-        <v>50</v>
+        <v>1.05</v>
       </c>
       <c r="AI51" s="1" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="AJ51" s="1" t="n">
         <v>4.98</v>
       </c>
     </row>
@@ -6273,13 +6274,13 @@
       <c r="AF52" s="2" t="n">
         <v>4.0794701986755</v>
       </c>
+      <c r="AG52" s="1" t="n">
+        <v>41</v>
+      </c>
       <c r="AH52" s="1" t="n">
-        <v>41</v>
+        <v>0.8</v>
       </c>
       <c r="AI52" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="AJ52" s="1" t="n">
         <v>0.68</v>
       </c>
     </row>
@@ -6380,13 +6381,13 @@
       <c r="AF53" s="2" t="n">
         <v>-0.291390728476821</v>
       </c>
+      <c r="AG53" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH53" s="1" t="n">
-        <v>50</v>
+        <v>4.16</v>
       </c>
       <c r="AI53" s="1" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="AJ53" s="1" t="n">
         <v>20.55</v>
       </c>
     </row>
@@ -6487,13 +6488,13 @@
       <c r="AF54" s="2" t="n">
         <v>2.88741721854305</v>
       </c>
+      <c r="AG54" s="1" t="n">
+        <v>70</v>
+      </c>
       <c r="AH54" s="1" t="n">
-        <v>70</v>
+        <v>-0.64</v>
       </c>
       <c r="AI54" s="1" t="n">
-        <v>-0.64</v>
-      </c>
-      <c r="AJ54" s="1" t="n">
         <v>-0.36</v>
       </c>
     </row>
@@ -6594,13 +6595,13 @@
       <c r="AF55" s="2" t="n">
         <v>6.19867549668874</v>
       </c>
+      <c r="AG55" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH55" s="1" t="n">
-        <v>49</v>
+        <v>3.51</v>
       </c>
       <c r="AI55" s="1" t="n">
-        <v>3.51</v>
-      </c>
-      <c r="AJ55" s="1" t="n">
         <v>29.48</v>
       </c>
     </row>
@@ -6701,13 +6702,13 @@
       <c r="AF56" s="2" t="n">
         <v>-1.74834437086093</v>
       </c>
+      <c r="AG56" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="AH56" s="1" t="n">
-        <v>48</v>
+        <v>0.29</v>
       </c>
       <c r="AI56" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="AJ56" s="1" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -6808,13 +6809,13 @@
       <c r="AF57" s="2" t="n">
         <v>0.503311258278146</v>
       </c>
+      <c r="AG57" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH57" s="1" t="n">
-        <v>51</v>
+        <v>-0.78</v>
       </c>
       <c r="AI57" s="1" t="n">
-        <v>-0.78</v>
-      </c>
-      <c r="AJ57" s="1" t="n">
         <v>-1.36</v>
       </c>
     </row>
@@ -6915,13 +6916,13 @@
       <c r="AF58" s="2" t="n">
         <v>3.28476821192053</v>
       </c>
+      <c r="AG58" s="1" t="n">
+        <v>55</v>
+      </c>
       <c r="AH58" s="1" t="n">
-        <v>55</v>
+        <v>-0.59</v>
       </c>
       <c r="AI58" s="1" t="n">
-        <v>-0.59</v>
-      </c>
-      <c r="AJ58" s="1" t="n">
         <v>0.18</v>
       </c>
     </row>
@@ -7022,13 +7023,13 @@
       <c r="AF59" s="2" t="n">
         <v>2.62251655629139</v>
       </c>
+      <c r="AG59" s="1" t="n">
+        <v>31</v>
+      </c>
       <c r="AH59" s="1" t="n">
-        <v>31</v>
+        <v>999</v>
       </c>
       <c r="AI59" s="1" t="n">
-        <v>999</v>
-      </c>
-      <c r="AJ59" s="1" t="n">
         <v>999</v>
       </c>
     </row>
@@ -7129,13 +7130,13 @@
       <c r="AF60" s="2" t="n">
         <v>3.81456953642384</v>
       </c>
+      <c r="AG60" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH60" s="1" t="n">
-        <v>47</v>
+        <v>0.2</v>
       </c>
       <c r="AI60" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AJ60" s="1" t="n">
         <v>0.68</v>
       </c>
     </row>
@@ -7236,13 +7237,13 @@
       <c r="AF61" s="2" t="n">
         <v>1.82781456953642</v>
       </c>
+      <c r="AG61" s="1" t="n">
+        <v>56</v>
+      </c>
       <c r="AH61" s="1" t="n">
-        <v>56</v>
+        <v>0.59</v>
       </c>
       <c r="AI61" s="1" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="AJ61" s="1" t="n">
         <v>2.14</v>
       </c>
     </row>
@@ -7343,13 +7344,13 @@
       <c r="AF62" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
+      <c r="AG62" s="1" t="n">
+        <v>52</v>
+      </c>
       <c r="AH62" s="1" t="n">
-        <v>52</v>
+        <v>0.46</v>
       </c>
       <c r="AI62" s="1" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="AJ62" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7450,13 +7451,13 @@
       <c r="AF63" s="2" t="n">
         <v>1.43046357615894</v>
       </c>
+      <c r="AG63" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH63" s="1" t="n">
-        <v>51</v>
+        <v>-1.46</v>
       </c>
       <c r="AI63" s="1" t="n">
-        <v>-1.46</v>
-      </c>
-      <c r="AJ63" s="1" t="n">
         <v>-2.62</v>
       </c>
     </row>
@@ -7557,13 +7558,13 @@
       <c r="AF64" s="2" t="n">
         <v>0.635761589403974</v>
       </c>
+      <c r="AG64" s="1" t="n">
+        <v>48</v>
+      </c>
       <c r="AH64" s="1" t="n">
-        <v>48</v>
+        <v>5.88</v>
       </c>
       <c r="AI64" s="1" t="n">
-        <v>5.88</v>
-      </c>
-      <c r="AJ64" s="1" t="n">
         <v>49.97</v>
       </c>
     </row>
@@ -7664,13 +7665,13 @@
       <c r="AF65" s="2" t="n">
         <v>3.01986754966887</v>
       </c>
+      <c r="AG65" s="1" t="n">
+        <v>36</v>
+      </c>
       <c r="AH65" s="1" t="n">
-        <v>36</v>
+        <v>-0.05</v>
       </c>
       <c r="AI65" s="1" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="AJ65" s="1" t="n">
         <v>1.78</v>
       </c>
     </row>
@@ -7771,13 +7772,13 @@
       <c r="AF66" s="2" t="n">
         <v>4.25116279069768</v>
       </c>
+      <c r="AG66" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH66" s="1" t="n">
-        <v>49</v>
+        <v>0.5</v>
       </c>
       <c r="AI66" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AJ66" s="1" t="n">
         <v>1.02</v>
       </c>
     </row>
@@ -7878,13 +7879,13 @@
       <c r="AF67" s="2" t="n">
         <v>-0.167441860465116</v>
       </c>
+      <c r="AG67" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH67" s="1" t="n">
-        <v>51</v>
+        <v>-0.05</v>
       </c>
       <c r="AI67" s="1" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="AJ67" s="1" t="n">
         <v>-0.36</v>
       </c>
     </row>
@@ -7985,13 +7986,13 @@
       <c r="AF68" s="2" t="n">
         <v>2.73953488372093</v>
       </c>
+      <c r="AG68" s="1" t="n">
+        <v>39</v>
+      </c>
       <c r="AH68" s="1" t="n">
-        <v>39</v>
+        <v>2.49</v>
       </c>
       <c r="AI68" s="1" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="AJ68" s="1" t="n">
         <v>8.24</v>
       </c>
     </row>
@@ -8092,13 +8093,13 @@
       <c r="AF69" s="2" t="n">
         <v>-1.33023255813954</v>
       </c>
+      <c r="AG69" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH69" s="1" t="n">
-        <v>51</v>
+        <v>1.78</v>
       </c>
       <c r="AI69" s="1" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="AJ69" s="1" t="n">
         <v>5.02</v>
       </c>
     </row>
@@ -8199,13 +8200,13 @@
       <c r="AF70" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
+      <c r="AG70" s="1" t="n">
+        <v>47</v>
+      </c>
       <c r="AH70" s="1" t="n">
-        <v>47</v>
+        <v>-0.22</v>
       </c>
       <c r="AI70" s="1" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="AJ70" s="1" t="n">
         <v>-0.23</v>
       </c>
     </row>
@@ -8306,13 +8307,13 @@
       <c r="AF71" s="2" t="n">
         <v>-0.516279069767442</v>
       </c>
+      <c r="AG71" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH71" s="1" t="n">
-        <v>50</v>
+        <v>-0.39</v>
       </c>
       <c r="AI71" s="1" t="n">
-        <v>-0.39</v>
-      </c>
-      <c r="AJ71" s="1" t="n">
         <v>0.94</v>
       </c>
     </row>
@@ -8413,13 +8414,13 @@
       <c r="AF72" s="2" t="n">
         <v>2.97209302325581</v>
       </c>
+      <c r="AG72" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH72" s="1" t="n">
-        <v>50</v>
+        <v>-1.07</v>
       </c>
       <c r="AI72" s="1" t="n">
-        <v>-1.07</v>
-      </c>
-      <c r="AJ72" s="1" t="n">
         <v>-0.85</v>
       </c>
     </row>
@@ -8520,13 +8521,13 @@
       <c r="AF73" s="2" t="n">
         <v>3.32093023255814</v>
       </c>
+      <c r="AG73" s="1" t="n">
+        <v>51</v>
+      </c>
       <c r="AH73" s="1" t="n">
-        <v>51</v>
+        <v>-0.95</v>
       </c>
       <c r="AI73" s="1" t="n">
-        <v>-0.95</v>
-      </c>
-      <c r="AJ73" s="1" t="n">
         <v>-0.32</v>
       </c>
     </row>
@@ -8627,13 +8628,13 @@
       <c r="AF74" s="2" t="n">
         <v>2.39069767441861</v>
       </c>
+      <c r="AG74" s="1" t="n">
+        <v>49</v>
+      </c>
       <c r="AH74" s="1" t="n">
-        <v>49</v>
+        <v>0.37</v>
       </c>
       <c r="AI74" s="1" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="AJ74" s="1" t="n">
         <v>0.13</v>
       </c>
     </row>
@@ -8734,13 +8735,13 @@
       <c r="AF75" s="2" t="n">
         <v>4.48372093023256</v>
       </c>
+      <c r="AG75" s="1" t="n">
+        <v>56</v>
+      </c>
       <c r="AH75" s="1" t="n">
-        <v>56</v>
+        <v>-1.24</v>
       </c>
       <c r="AI75" s="1" t="n">
-        <v>-1.24</v>
-      </c>
-      <c r="AJ75" s="1" t="n">
         <v>-1.04</v>
       </c>
     </row>
@@ -8841,13 +8842,13 @@
       <c r="AF76" s="2" t="n">
         <v>-0.0511627906976746</v>
       </c>
+      <c r="AG76" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="AH76" s="1" t="n">
-        <v>59</v>
+        <v>1.04</v>
       </c>
       <c r="AI76" s="1" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="AJ76" s="1" t="n">
         <v>3.4</v>
       </c>
     </row>
@@ -8948,13 +8949,13 @@
       <c r="AF77" s="2" t="n">
         <v>1.57674418604651</v>
       </c>
+      <c r="AG77" s="1" t="n">
+        <v>34</v>
+      </c>
       <c r="AH77" s="1" t="n">
-        <v>34</v>
+        <v>-0.47</v>
       </c>
       <c r="AI77" s="1" t="n">
-        <v>-0.47</v>
-      </c>
-      <c r="AJ77" s="1" t="n">
         <v>2.76</v>
       </c>
     </row>
@@ -9055,13 +9056,13 @@
       <c r="AF78" s="2" t="n">
         <v>999</v>
       </c>
+      <c r="AG78" s="1" t="n">
+        <v>35</v>
+      </c>
       <c r="AH78" s="1" t="n">
-        <v>35</v>
+        <v>0.23</v>
       </c>
       <c r="AI78" s="1" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="AJ78" s="1" t="n">
         <v>1.27</v>
       </c>
     </row>
@@ -9162,13 +9163,13 @@
       <c r="AF79" s="2" t="n">
         <v>-0.4</v>
       </c>
+      <c r="AG79" s="1" t="n">
+        <v>999</v>
+      </c>
       <c r="AH79" s="1" t="n">
         <v>999</v>
       </c>
       <c r="AI79" s="1" t="n">
-        <v>999</v>
-      </c>
-      <c r="AJ79" s="1" t="n">
         <v>999</v>
       </c>
     </row>
@@ -9269,13 +9270,13 @@
       <c r="AF80" s="2" t="n">
         <v>-1.67906976744186</v>
       </c>
+      <c r="AG80" s="1" t="n">
+        <v>45</v>
+      </c>
       <c r="AH80" s="1" t="n">
-        <v>45</v>
+        <v>0.02</v>
       </c>
       <c r="AI80" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AJ80" s="1" t="n">
         <v>-0.25</v>
       </c>
     </row>
@@ -9376,13 +9377,13 @@
       <c r="AF81" s="2" t="n">
         <v>2.38156359393232</v>
       </c>
+      <c r="AG81" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AH81" s="1" t="n">
-        <v>50</v>
+        <v>1.42</v>
       </c>
       <c r="AI81" s="1" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="AJ81" s="1" t="n">
         <v>3.14</v>
       </c>
     </row>
@@ -9483,13 +9484,13 @@
       <c r="AF82" s="2" t="n">
         <v>-0.283720930232558</v>
       </c>
+      <c r="AG82" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="AH82" s="1" t="n">
-        <v>59</v>
+        <v>-0.06</v>
       </c>
       <c r="AI82" s="1" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="AJ82" s="1" t="n">
         <v>-0.19</v>
       </c>
     </row>
@@ -9590,13 +9591,13 @@
       <c r="AF83" s="2" t="n">
         <v>1.16556291390729</v>
       </c>
+      <c r="AG83" s="1" t="n">
+        <v>39</v>
+      </c>
       <c r="AH83" s="1" t="n">
-        <v>39</v>
+        <v>1.07</v>
       </c>
       <c r="AI83" s="1" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="AJ83" s="1" t="n">
         <v>1.69</v>
       </c>
     </row>
@@ -12048,12 +12049,6 @@
       </c>
       <c r="AF108" s="2" t="n">
         <v>0.646511627906977</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E112" s="1" t="n">
-        <f aca="false">E107+E80</f>
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>